<commit_message>
working on edits to KI figure following the meeting today
</commit_message>
<xml_diff>
--- a/data/Platy_15c-vrs-15d.xlsx
+++ b/data/Platy_15c-vrs-15d.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="6660" windowWidth="28160" windowHeight="11340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="11260" windowWidth="28160" windowHeight="6660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -150,24 +150,24 @@
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,10 +448,14 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -459,21 +463,21 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="8" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -485,7 +489,7 @@
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -497,7 +501,7 @@
       <c r="G4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -506,10 +510,10 @@
       <c r="J4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="8" t="s">
         <v>11</v>
       </c>
     </row>
@@ -517,37 +521,37 @@
       <c r="A5">
         <v>8</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <v>13</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="4">
         <v>7</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="3">
         <f>SUM(B5:D5)</f>
         <v>21</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
         <f>(C5/E5)*100</f>
         <v>61.904761904761905</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="3">
         <f>(B5/E5)*100</f>
         <v>4.7619047619047619</v>
       </c>
-      <c r="H5" s="10">
-        <v>0</v>
-      </c>
-      <c r="I5" s="5">
+      <c r="H5" s="7">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
         <v>14</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="3">
         <v>1</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="3">
         <f>SUM(H5:J5)</f>
         <v>15</v>
       </c>
@@ -563,37 +567,37 @@
       <c r="A6">
         <v>35</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="3">
         <v>23</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>16</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="4">
         <v>6</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="3">
         <f t="shared" ref="E6:E8" si="0">SUM(B6:D6)</f>
         <v>45</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="3">
         <f t="shared" ref="F6:F8" si="1">(C6/E6)*100</f>
         <v>35.555555555555557</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="3">
         <f>(B6/E6)*100</f>
         <v>51.111111111111107</v>
       </c>
-      <c r="H6" s="10">
-        <v>0</v>
-      </c>
-      <c r="I6" s="5">
+      <c r="H6" s="7">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
         <v>15</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="3">
         <v>1</v>
       </c>
-      <c r="K6" s="5">
+      <c r="K6" s="3">
         <f t="shared" ref="K6:K8" si="2">SUM(H6:J6)</f>
         <v>16</v>
       </c>
@@ -609,35 +613,35 @@
       <c r="A7">
         <v>27</v>
       </c>
-      <c r="B7" s="5">
-        <v>0</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0</v>
-      </c>
-      <c r="D7" s="6">
-        <v>0</v>
-      </c>
-      <c r="E7" s="5">
+      <c r="B7" s="3">
+        <v>0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F7" s="5">
-        <v>0</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0</v>
-      </c>
-      <c r="H7" s="10">
-        <v>0</v>
-      </c>
-      <c r="I7" s="5">
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="3">
         <v>1</v>
       </c>
-      <c r="J7" s="5">
-        <v>0</v>
-      </c>
-      <c r="K7" s="5">
+      <c r="J7" s="3">
+        <v>0</v>
+      </c>
+      <c r="K7" s="3">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -650,37 +654,37 @@
       <c r="A8">
         <v>32</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="3">
         <v>1</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="3">
         <v>3</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="4">
         <v>1</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="3">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="G8" s="5">
+      <c r="G8" s="3">
         <f>(B8/E8)*100</f>
         <v>20</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="7">
         <v>2</v>
       </c>
-      <c r="I8" s="5">
+      <c r="I8" s="3">
         <v>5</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K8" s="5">
+      <c r="K8" s="3">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
@@ -690,152 +694,152 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>